<commit_message>
first transformations to CPSV-AP
</commit_message>
<xml_diff>
--- a/source-data/dataSpain.XLSX
+++ b/source-data/dataSpain.XLSX
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombeura\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vandeloc\Documents\Documents\CoS\Pilot - PortugalSpain data transform\Github - Data transformation\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="0" windowWidth="23715" windowHeight="10035"/>
+    <workbookView xWindow="-30" yWindow="0" windowWidth="23715" windowHeight="10035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SDG Proposal" sheetId="1" r:id="rId1"/>
@@ -680,9 +680,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>es</t>
-  </si>
-  <si>
     <t>Certificado de residente</t>
   </si>
   <si>
@@ -1559,6 +1556,9 @@
 How?
 Enter the Electronic Office of the Ministry of Justice and access the Birth Certificate.
 You can choose to receive the certificate by postal mail at the address indicated in the application or pick it up in the corresponding Civil Registry that you expressly indicate. In this case the Civil Registry will tell you the date from which you can collect it from.</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
 </sst>
 </file>
@@ -2511,7 +2511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
@@ -3146,10 +3146,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F11" s="34" t="s">
         <v>132</v>
@@ -3817,10 +3817,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,10 +3934,10 @@
         <v>146</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>150</v>
@@ -3958,7 +3958,7 @@
         <v>163</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N3" s="18" t="s">
         <v>0</v>
@@ -3979,34 +3979,34 @@
         <v>994455</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>168</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>169</v>
       </c>
       <c r="I4" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>156</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="120" x14ac:dyDescent="0.25">
@@ -4018,34 +4018,34 @@
         <v>203557</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G5" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>180</v>
-      </c>
       <c r="H5" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I5" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>156</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="150" x14ac:dyDescent="0.25">
@@ -4057,46 +4057,46 @@
         <v>200265</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>184</v>
-      </c>
       <c r="F6" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K6" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N6" s="17" t="s">
         <v>0</v>
       </c>
       <c r="O6" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -4108,34 +4108,34 @@
         <v>20650</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G7" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="25" t="s">
+      <c r="H7" s="17" t="s">
         <v>193</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>194</v>
       </c>
       <c r="I7" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K7" s="25" t="s">
         <v>156</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="120" x14ac:dyDescent="0.25">
@@ -4147,34 +4147,34 @@
         <v>203508</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G8" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="I8" s="52" t="s">
+        <v>305</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="I8" s="52" t="s">
-        <v>306</v>
-      </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="K8" s="25" t="s">
-        <v>205</v>
-      </c>
       <c r="P8" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="150" x14ac:dyDescent="0.25">
@@ -4186,31 +4186,31 @@
         <v>203888</v>
       </c>
       <c r="C9" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="E9" s="17" t="s">
+      <c r="I9" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>212</v>
-      </c>
       <c r="K9" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -4222,31 +4222,31 @@
         <v>220359</v>
       </c>
       <c r="C10" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>215</v>
-      </c>
       <c r="K10" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="255" x14ac:dyDescent="0.25">
@@ -4258,28 +4258,28 @@
         <v>208249</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="F11" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G11" s="25" t="s">
+      <c r="H11" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="I11" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="J11" s="19" t="s">
         <v>226</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>227</v>
       </c>
       <c r="K11" s="25" t="s">
         <v>156</v>
@@ -4294,31 +4294,31 @@
         <v>215091</v>
       </c>
       <c r="C12" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="H12" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="I12" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="J12" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>233</v>
-      </c>
       <c r="K12" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -4330,34 +4330,34 @@
         <v>203212</v>
       </c>
       <c r="C13" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F13" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G13" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13" s="25" t="s">
+      <c r="H13" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="I13" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="J13" s="19" t="s">
         <v>239</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>240</v>
       </c>
       <c r="K13" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="360" x14ac:dyDescent="0.25">
@@ -4369,31 +4369,31 @@
         <v>219231</v>
       </c>
       <c r="C14" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="H14" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="H14" s="17" t="s">
+      <c r="I14" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="J14" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J14" s="19" t="s">
-        <v>245</v>
-      </c>
       <c r="K14" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="120" x14ac:dyDescent="0.25">
@@ -4405,31 +4405,31 @@
         <v>209380</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="H15" s="17" t="s">
+      <c r="I15" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="J15" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="J15" s="19" t="s">
-        <v>251</v>
-      </c>
       <c r="K15" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -4441,31 +4441,31 @@
         <v>210076</v>
       </c>
       <c r="C16" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="H16" s="17" t="s">
+      <c r="I16" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="J16" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="J16" s="19" t="s">
-        <v>258</v>
-      </c>
       <c r="K16" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -4477,31 +4477,31 @@
         <v>213956</v>
       </c>
       <c r="C17" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="F17" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="H17" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="H17" s="17" t="s">
+      <c r="I17" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="J17" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="J17" s="19" t="s">
-        <v>267</v>
-      </c>
       <c r="K17" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -4513,31 +4513,31 @@
         <v>206916</v>
       </c>
       <c r="C18" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="F18" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="H18" s="17" t="s">
+      <c r="I18" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="J18" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="J18" s="19" t="s">
-        <v>273</v>
-      </c>
       <c r="K18" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="27" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4549,31 +4549,31 @@
         <v>210078</v>
       </c>
       <c r="C19" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="E19" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="F19" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="J19" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>278</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="I19" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>277</v>
-      </c>
       <c r="K19" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O19" s="29"/>
     </row>
@@ -4586,31 +4586,31 @@
         <v>221166</v>
       </c>
       <c r="C20" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="F20" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G20" s="25" t="s">
         <v>343</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G20" s="25" t="s">
+      <c r="H20" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="J20" s="19" t="s">
+      <c r="K20" s="25" t="s">
         <v>345</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -4622,28 +4622,28 @@
         <v>287471</v>
       </c>
       <c r="C21" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="H21" s="17" t="s">
         <v>347</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G21" s="25" t="s">
+      <c r="I21" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="J21" s="19" t="s">
         <v>351</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>352</v>
       </c>
       <c r="K21" s="25" t="s">
         <v>156</v>
@@ -4658,34 +4658,34 @@
         <v>202057</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="F22" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="H22" s="17" t="s">
         <v>355</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>351</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>356</v>
       </c>
       <c r="I22" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K22" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -4697,34 +4697,34 @@
         <v>994715</v>
       </c>
       <c r="C23" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>358</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="E23" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="F23" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G23" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="F23" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G23" s="25" t="s">
+      <c r="H23" s="17" t="s">
         <v>361</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>362</v>
       </c>
       <c r="I23" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K23" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -4736,34 +4736,34 @@
         <v>997046</v>
       </c>
       <c r="C24" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>366</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="F24" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>367</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>368</v>
       </c>
       <c r="I24" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K24" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -4775,31 +4775,31 @@
         <v>219601</v>
       </c>
       <c r="C25" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="E25" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="F25" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="J25" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="F25" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>379</v>
-      </c>
       <c r="K25" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="165" x14ac:dyDescent="0.25">
@@ -4811,28 +4811,28 @@
         <v>214599</v>
       </c>
       <c r="C26" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="E26" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="F26" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="J26" s="19" t="s">
         <v>374</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="J26" s="19" t="s">
-        <v>375</v>
       </c>
       <c r="K26" s="25" t="s">
         <v>156</v>
@@ -4847,31 +4847,31 @@
         <v>205767</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="E27" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>381</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="I27" s="25" t="s">
         <v>383</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>382</v>
-      </c>
-      <c r="I27" s="25" t="s">
+      <c r="J27" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="J27" s="19" t="s">
-        <v>385</v>
-      </c>
       <c r="K27" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -4883,34 +4883,34 @@
         <v>992253</v>
       </c>
       <c r="C28" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="E28" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="F28" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G28" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="F28" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" s="25" t="s">
+      <c r="H28" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="I28" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K28" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -4922,34 +4922,34 @@
         <v>992224</v>
       </c>
       <c r="C29" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="D29" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="E29" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>395</v>
-      </c>
       <c r="F29" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G29" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="H29" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="I29" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J29" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="K29" s="25" t="s">
         <v>396</v>
       </c>
-      <c r="K29" s="25" t="s">
-        <v>397</v>
-      </c>
       <c r="L29" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4961,34 +4961,34 @@
         <v>997800</v>
       </c>
       <c r="C30" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="E30" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="H30" s="17" t="s">
         <v>401</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>404</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>402</v>
       </c>
       <c r="I30" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K30" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -5000,34 +5000,34 @@
         <v>992225</v>
       </c>
       <c r="C31" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="E31" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="F31" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G31" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="H31" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="I31" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J31" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="K31" s="25" t="s">
         <v>396</v>
       </c>
-      <c r="K31" s="25" t="s">
+      <c r="L31" s="17" t="s">
         <v>397</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -5039,34 +5039,34 @@
         <v>992257</v>
       </c>
       <c r="C32" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>409</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="E32" s="17" t="s">
         <v>410</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>411</v>
-      </c>
       <c r="F32" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G32" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="H32" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="I32" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K32" s="25" t="s">
         <v>156</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -5119,10 +5119,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5145,7 +5145,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B1" s="59" t="s">
         <v>151</v>
@@ -5236,19 +5236,19 @@
         <v>Bithday Certificate</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>449</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>280</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>281</v>
       </c>
       <c r="I3" s="47" t="s">
         <v>144</v>
@@ -5257,22 +5257,22 @@
         <v>157</v>
       </c>
       <c r="K3" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L3" s="21" t="s">
         <v>163</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="O3" s="40" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -5288,31 +5288,31 @@
         <v>Residence Certificate for Europeans</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>310</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I4" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K4" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -5328,31 +5328,31 @@
         <v>Application for European Health Insurance Card</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>312</v>
-      </c>
       <c r="F5" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I5" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K5" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -5368,43 +5368,43 @@
         <v>Communication of change of address</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>314</v>
-      </c>
       <c r="F6" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I6" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K6" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N6" s="17" t="s">
         <v>0</v>
       </c>
       <c r="O6" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -5420,31 +5420,31 @@
         <v>Claiming retirement pension</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>316</v>
-      </c>
       <c r="F7" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I7" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K7" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="150" x14ac:dyDescent="0.25">
@@ -5460,28 +5460,28 @@
         <v>Instalación de situados para ejercer la venta ambulante</v>
       </c>
       <c r="D8" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>318</v>
-      </c>
       <c r="F8" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I8" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K8" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -5497,28 +5497,28 @@
         <v xml:space="preserve">Authorization request for operating Fish Farms or Aquaculture Facilities </v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>320</v>
-      </c>
       <c r="F9" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K9" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -5534,28 +5534,28 @@
         <v>Authorization of commercial license to large commercial establishments and shopping centers.</v>
       </c>
       <c r="D10" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>322</v>
-      </c>
       <c r="F10" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K10" s="47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="210" x14ac:dyDescent="0.25">
@@ -5571,28 +5571,28 @@
         <v xml:space="preserve">Registry for startup of a guesthouse activity </v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>324</v>
-      </c>
       <c r="F11" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H11" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="J11" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="J11" s="19" t="s">
-        <v>227</v>
-      </c>
       <c r="K11" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -5608,28 +5608,28 @@
         <v>Communication of cessation of activity of a non-hotel tourist accommodation establishment</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>326</v>
-      </c>
       <c r="F12" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H12" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="I12" s="47" t="s">
         <v>229</v>
       </c>
-      <c r="I12" s="47" t="s">
-        <v>230</v>
-      </c>
       <c r="J12" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K12" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="150" x14ac:dyDescent="0.25">
@@ -5645,31 +5645,31 @@
         <v>Start of activity of catering facility</v>
       </c>
       <c r="D13" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>328</v>
-      </c>
       <c r="F13" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H13" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="47" t="s">
         <v>238</v>
       </c>
-      <c r="I13" s="47" t="s">
+      <c r="J13" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="J13" s="19" t="s">
-        <v>240</v>
-      </c>
       <c r="K13" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="315" x14ac:dyDescent="0.25">
@@ -5685,28 +5685,28 @@
         <v>Register of Real Estate Agents of Catalonia</v>
       </c>
       <c r="D14" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>330</v>
-      </c>
       <c r="F14" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H14" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="I14" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="J14" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J14" s="19" t="s">
-        <v>245</v>
-      </c>
       <c r="K14" s="47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="120" x14ac:dyDescent="0.25">
@@ -5722,28 +5722,28 @@
         <v>Clearance sales communication</v>
       </c>
       <c r="D15" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>332</v>
-      </c>
       <c r="F15" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H15" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="I15" s="47" t="s">
         <v>249</v>
       </c>
-      <c r="I15" s="47" t="s">
+      <c r="J15" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="J15" s="19" t="s">
-        <v>251</v>
-      </c>
       <c r="K15" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -5759,28 +5759,28 @@
         <v>Registration in the Special Register of Repair Shops for motor vehicles and their equipment and components</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H16" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="I16" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="I16" s="47" t="s">
+      <c r="J16" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="J16" s="19" t="s">
-        <v>258</v>
-      </c>
       <c r="K16" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -5796,28 +5796,28 @@
         <v>Registration in the Official Register of tanning centers</v>
       </c>
       <c r="D17" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>336</v>
-      </c>
       <c r="F17" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H17" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="I17" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="I17" s="47" t="s">
+      <c r="J17" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="J17" s="19" t="s">
-        <v>267</v>
-      </c>
       <c r="K17" s="47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -5833,28 +5833,28 @@
         <v>Sanitary authorization for tattoo and piercing establishments</v>
       </c>
       <c r="D18" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>337</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>338</v>
-      </c>
       <c r="F18" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H18" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="I18" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="J18" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="J18" s="19" t="s">
-        <v>273</v>
-      </c>
       <c r="K18" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="27" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5870,28 +5870,28 @@
         <v>Business licence for large retail trade establishment</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>339</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>166</v>
+        <v>338</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>449</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H19" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="I19" s="49" t="s">
         <v>256</v>
       </c>
-      <c r="I19" s="49" t="s">
-        <v>257</v>
-      </c>
       <c r="J19" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K19" s="49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O19" s="29"/>
     </row>
@@ -5908,28 +5908,28 @@
         <v>Study aids to produce doctoral thesis</v>
       </c>
       <c r="D20" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>425</v>
-      </c>
       <c r="F20" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I20" s="47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K20" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -5945,28 +5945,28 @@
         <v>Application for Grade or Master studies in Granada University</v>
       </c>
       <c r="D21" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>426</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>427</v>
-      </c>
       <c r="F21" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I21" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K21" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -5982,31 +5982,31 @@
         <v>Homologation of university degrees and recognition of qualifications</v>
       </c>
       <c r="D22" s="17" t="s">
+        <v>427</v>
+      </c>
+      <c r="E22" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>429</v>
-      </c>
       <c r="F22" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I22" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K22" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -6022,31 +6022,31 @@
         <v>Modification of data about pension</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>429</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>430</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>431</v>
-      </c>
       <c r="F23" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I23" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K23" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -6065,28 +6065,28 @@
         <v>86</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I24" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K24" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="120" x14ac:dyDescent="0.25">
@@ -6102,28 +6102,28 @@
         <v>Declaration of prices and services of tourist accommodation</v>
       </c>
       <c r="D25" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="E25" s="17" t="s">
-        <v>434</v>
-      </c>
       <c r="F25" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H25" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="I25" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="I25" s="47" t="s">
-        <v>244</v>
-      </c>
       <c r="J25" s="19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K25" s="47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="225" x14ac:dyDescent="0.25">
@@ -6139,28 +6139,28 @@
         <v xml:space="preserve">Change of activity in business premises </v>
       </c>
       <c r="D26" s="17" t="s">
+        <v>434</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="E26" s="17" t="s">
-        <v>436</v>
-      </c>
       <c r="F26" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H26" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="I26" s="47" t="s">
         <v>238</v>
       </c>
-      <c r="I26" s="47" t="s">
-        <v>239</v>
-      </c>
       <c r="J26" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K26" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -6176,28 +6176,28 @@
         <v>Business licence for arcade establishment</v>
       </c>
       <c r="D27" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>437</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>438</v>
-      </c>
       <c r="F27" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I27" s="47" t="s">
+        <v>383</v>
+      </c>
+      <c r="J27" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="J27" s="19" t="s">
-        <v>385</v>
-      </c>
       <c r="K27" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -6213,31 +6213,31 @@
         <v>Employer registration in Social Security with tax account code</v>
       </c>
       <c r="D28" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>440</v>
-      </c>
       <c r="F28" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I28" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K28" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P28" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -6253,31 +6253,31 @@
         <v>Registration of workers in the General Scheme</v>
       </c>
       <c r="D29" s="17" t="s">
+        <v>440</v>
+      </c>
+      <c r="E29" s="17" t="s">
         <v>441</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>442</v>
-      </c>
       <c r="F29" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I29" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K29" s="47" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P29" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -6293,31 +6293,31 @@
         <v>Submmition of Corporate Tax (Model 200)</v>
       </c>
       <c r="D30" s="17" t="s">
+        <v>442</v>
+      </c>
+      <c r="E30" s="17" t="s">
         <v>443</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>444</v>
-      </c>
       <c r="F30" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I30" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K30" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -6333,31 +6333,31 @@
         <v>Withdrawal of workers in the General Scheme</v>
       </c>
       <c r="D31" s="17" t="s">
+        <v>444</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>446</v>
-      </c>
       <c r="F31" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I31" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K31" s="47" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P31" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -6373,31 +6373,31 @@
         <v>Payment of social security contributions for workers in the General Scheme</v>
       </c>
       <c r="D32" s="17" t="s">
+        <v>446</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>448</v>
-      </c>
       <c r="F32" s="17" t="s">
-        <v>166</v>
+        <v>449</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I32" s="47" t="s">
         <v>144</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K32" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P32" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>